<commit_message>
Build more of program skeleton
</commit_message>
<xml_diff>
--- a/PhotonManager_Requirments.xlsx
+++ b/PhotonManager_Requirments.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhotonLaserTagManager\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mylisa\Documents\GitHub\PhotonLaserTagManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35ADFFF-D157-4815-8BF4-8487C5D2B8A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4177F2-6C5D-4BBC-A9F7-B811FF0D2102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D1978DAF-1EAF-4D70-9253-8005321C1CD1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D1978DAF-1EAF-4D70-9253-8005321C1CD1}"/>
   </bookViews>
   <sheets>
-    <sheet name="High Level Requirements" sheetId="2" r:id="rId1"/>
-    <sheet name="Low Level Requirements" sheetId="1" r:id="rId2"/>
+    <sheet name="HighLevelRequirements" sheetId="2" r:id="rId1"/>
+    <sheet name="LowLevelRequirements" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Laser Tag System High-Level Requirments</t>
   </si>
@@ -51,22 +51,31 @@
     <t>Laser Tag System Low-Level Requirments</t>
   </si>
   <si>
-    <t xml:space="preserve">TODO: Bubble/Flow chart </t>
+    <t>Parent HLR Trace</t>
   </si>
   <si>
-    <t>Trace to HLR</t>
+    <t>Link to HLR</t>
   </si>
   <si>
-    <t>The Photon Laser Tag Manager System Shall be displayed in a single, resizable, window.</t>
+    <t>The Photon Laser Tag Manager System (PLTMS) shall be displayed in a single, resizable, window.</t>
   </si>
   <si>
-    <t>4</t>
+    <t>The PLTMS shall process user mouse and keyboard inputs to interact and manage the use of the program.</t>
   </si>
   <si>
-    <t>The Photon Laser Tag Manager System shall have a resizable window, with a minimum size of (XXXX x XXXX) pixels</t>
+    <t>The Photon Laser Tag Manager System (PLTMS) shall update the display window every 12 milliseconds (83.3Hz) in a non-blocking fashion.</t>
   </si>
   <si>
-    <t>The Photon Laser Tag Manager System shall update the display window every 12 milliseconds (83.3Hz)</t>
+    <t>The PLTMS shall have a resizable window, with a minimum size of (XXXX x XXXX) pixels</t>
+  </si>
+  <si>
+    <t>The PLTMS shall use user keyboard inputs to fill selected text fields in the team selection screen</t>
+  </si>
+  <si>
+    <t>Reminder</t>
+  </si>
+  <si>
+    <t>Low Level Requirements are the only requirements that should be tagged in code. High level requirements usually get tagged in system-level tests. (If we do any for this project that aren't manual tests)</t>
   </si>
 </sst>
 </file>
@@ -133,7 +142,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -215,12 +224,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -252,42 +298,140 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -312,40 +456,6 @@
           <color indexed="64"/>
         </left>
         <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -586,23 +696,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{075AD733-E70C-4BB1-93AC-CA78B944AF5C}" name="Table13" displayName="Table13" ref="B3:C50" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
-  <autoFilter ref="B3:C50" xr:uid="{F9BD3E6F-18DE-4847-AC23-6689F47F21BF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{075AD733-E70C-4BB1-93AC-CA78B944AF5C}" name="Table13" displayName="Table13" ref="B3:C100" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
+  <autoFilter ref="B3:C100" xr:uid="{F9BD3E6F-18DE-4847-AC23-6689F47F21BF}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{FE64C739-08B3-4B4F-AED7-A9DD200A1698}" name="Requirement Number" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{32A148A2-D59A-4A68-9464-2994A965C0DE}" name="Requirement Text" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{FE64C739-08B3-4B4F-AED7-A9DD200A1698}" name="Requirement Number" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{32A148A2-D59A-4A68-9464-2994A965C0DE}" name="Requirement Text" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F9BD3E6F-18DE-4847-AC23-6689F47F21BF}" name="Table1" displayName="Table1" ref="B3:D50" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="B3:D50" xr:uid="{F9BD3E6F-18DE-4847-AC23-6689F47F21BF}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{54BA2B99-7968-4EF6-ABC0-D386B3BCB17C}" name="Requirement Number" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{1886CC6A-5D0D-42D3-BA80-3C2354B9499A}" name="Requirement Text" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{58DD8FAE-AA59-421D-A898-98D160A6E28A}" name="Trace to HLR" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F9BD3E6F-18DE-4847-AC23-6689F47F21BF}" name="Table1" displayName="Table1" ref="B3:E100" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="B3:E100" xr:uid="{F9BD3E6F-18DE-4847-AC23-6689F47F21BF}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{54BA2B99-7968-4EF6-ABC0-D386B3BCB17C}" name="Requirement Number" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{1886CC6A-5D0D-42D3-BA80-3C2354B9499A}" name="Requirement Text" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{58DD8FAE-AA59-421D-A898-98D160A6E28A}" name="Parent HLR Trace" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{B8725959-29DD-4866-80D9-56BA64BCFA81}" name="Link to HLR" dataDxfId="1">
+      <calculatedColumnFormula>IF(ISBLANK(D4),"",HYPERLINK("#'HighLevelRequirements'!B"&amp;D4,"Link"))</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -925,31 +1038,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A0FAC97-098D-4BD2-9CE1-5FB4D603BBAA}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" style="10" customWidth="1"/>
-    <col min="3" max="3" width="68.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="25.85546875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="68.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="8"/>
     </row>
-    <row r="2" spans="2:3" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B2" s="11" t="s">
+    <row r="2" spans="2:11" ht="24" x14ac:dyDescent="0.4">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
-    </row>
-    <row r="3" spans="2:3" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="17"/>
+    </row>
+    <row r="3" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -957,7 +1073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="36" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11" ht="37.5" x14ac:dyDescent="0.3">
       <c r="B4" s="9">
         <f>IF(ISBLANK(C4), "", ROW(B4))</f>
         <v>4</v>
@@ -966,331 +1082,574 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B5" s="9" t="str">
+    <row r="5" spans="2:11" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B5" s="9">
         <f t="shared" ref="B5:B50" si="0">IF(ISBLANK(C5), "", ROW(B5))</f>
-        <v/>
-      </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+    </row>
+    <row r="6" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="G6" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C16" s="4"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C19" s="4"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C20" s="4"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C21" s="4"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C23" s="4"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C26" s="4"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C31" s="4"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C32" s="4"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C36" s="4"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C41" s="4"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B42" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C42" s="4"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C43" s="4"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B46" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B47" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C47" s="4"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B48" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C48" s="4"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C49" s="4"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" s="9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C50" s="7"/>
     </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="9"/>
+      <c r="C51" s="7"/>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B52" s="9"/>
+      <c r="C52" s="7"/>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="9"/>
+      <c r="C53" s="7"/>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="9"/>
+      <c r="C54" s="7"/>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B55" s="9"/>
+      <c r="C55" s="7"/>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B56" s="9"/>
+      <c r="C56" s="7"/>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B57" s="9"/>
+      <c r="C57" s="7"/>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B58" s="9"/>
+      <c r="C58" s="7"/>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B59" s="9"/>
+      <c r="C59" s="7"/>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B60" s="9"/>
+      <c r="C60" s="7"/>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B61" s="9"/>
+      <c r="C61" s="7"/>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B62" s="9"/>
+      <c r="C62" s="7"/>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B63" s="9"/>
+      <c r="C63" s="7"/>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B64" s="9"/>
+      <c r="C64" s="7"/>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B65" s="9"/>
+      <c r="C65" s="7"/>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B66" s="9"/>
+      <c r="C66" s="7"/>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B67" s="9"/>
+      <c r="C67" s="7"/>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B68" s="9"/>
+      <c r="C68" s="7"/>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B69" s="9"/>
+      <c r="C69" s="7"/>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B70" s="9"/>
+      <c r="C70" s="7"/>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B71" s="9"/>
+      <c r="C71" s="7"/>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B72" s="9"/>
+      <c r="C72" s="7"/>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B73" s="9"/>
+      <c r="C73" s="7"/>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B74" s="9"/>
+      <c r="C74" s="7"/>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B75" s="9"/>
+      <c r="C75" s="7"/>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B76" s="9"/>
+      <c r="C76" s="7"/>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B77" s="9"/>
+      <c r="C77" s="7"/>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B78" s="9"/>
+      <c r="C78" s="7"/>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B79" s="9"/>
+      <c r="C79" s="7"/>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B80" s="9"/>
+      <c r="C80" s="7"/>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B81" s="9"/>
+      <c r="C81" s="7"/>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B82" s="9"/>
+      <c r="C82" s="7"/>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B83" s="9"/>
+      <c r="C83" s="7"/>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B84" s="9"/>
+      <c r="C84" s="7"/>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B85" s="9"/>
+      <c r="C85" s="7"/>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B86" s="9"/>
+      <c r="C86" s="7"/>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B87" s="9"/>
+      <c r="C87" s="7"/>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B88" s="9"/>
+      <c r="C88" s="7"/>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B89" s="9"/>
+      <c r="C89" s="7"/>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B90" s="9"/>
+      <c r="C90" s="7"/>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B91" s="9"/>
+      <c r="C91" s="7"/>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B92" s="9"/>
+      <c r="C92" s="7"/>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B93" s="9"/>
+      <c r="C93" s="7"/>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B94" s="9"/>
+      <c r="C94" s="7"/>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B95" s="9"/>
+      <c r="C95" s="7"/>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B96" s="9"/>
+      <c r="C96" s="7"/>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B97" s="9"/>
+      <c r="C97" s="7"/>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B98" s="9"/>
+      <c r="C98" s="7"/>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B99" s="9"/>
+      <c r="C99" s="7"/>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B100" s="9"/>
+      <c r="C100" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="G6:K11"/>
+    <mergeCell ref="G5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1302,441 +1661,1087 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65AA9B14-2284-4462-952A-49E69BC5ADF4}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" style="10" customWidth="1"/>
-    <col min="3" max="3" width="68.33203125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="2"/>
-    <col min="6" max="6" width="38.6640625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="25.85546875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="68.28515625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="19" style="12" customWidth="1"/>
+    <col min="6" max="6" width="38.7109375" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="8"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="13"/>
-    </row>
-    <row r="2" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B2" s="11" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="2:6" ht="24" x14ac:dyDescent="0.4">
+      <c r="B2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="11"/>
-    </row>
-    <row r="3" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="17"/>
+    </row>
+    <row r="3" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="36" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:6" ht="56.25" x14ac:dyDescent="0.3">
       <c r="B4" s="9">
         <f>IF(ISBLANK(C4), "", ROW(B4))</f>
         <v>4</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="26">
+        <v>4</v>
+      </c>
+      <c r="E4" s="18" t="str">
+        <f t="shared" ref="E4:E50" si="0">IF(ISBLANK(D4),"",HYPERLINK("#'HighLevelRequirements'!B"&amp;D4,"Link"))</f>
+        <v>Link</v>
+      </c>
+      <c r="F4" s="20"/>
+    </row>
+    <row r="5" spans="2:6" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B5" s="9">
+        <f t="shared" ref="B5:B68" si="1">IF(ISBLANK(C5), "", ROW(B5))</f>
+        <v>5</v>
+      </c>
+      <c r="C5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="36" x14ac:dyDescent="0.35">
-      <c r="B5" s="9">
-        <f t="shared" ref="B5:B50" si="0">IF(ISBLANK(C5), "", ROW(B5))</f>
+      <c r="D5" s="27">
+        <v>4</v>
+      </c>
+      <c r="E5" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B6" s="9">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="25">
         <v>5</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B6" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="12"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E6" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="12"/>
-      <c r="F7" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="21">
+        <v>40</v>
+      </c>
+      <c r="E8" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="12"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="12"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="12"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="12"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="12"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="12"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="12"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="12"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="12"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="12"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="12"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="12"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="12"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="12"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="12"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="12"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="12"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="12"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="12"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="12"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="12"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="12"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="12"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="12"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="12"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="12"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="12"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C39" s="18"/>
-      <c r="D39" s="12"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="12"/>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C41" s="18"/>
-      <c r="D41" s="12"/>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C42" s="18"/>
-      <c r="D42" s="12"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C43" s="18"/>
-      <c r="D43" s="12"/>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C43" s="14"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B44" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C44" s="18"/>
-      <c r="D44" s="12"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B45" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C45" s="18"/>
-      <c r="D45" s="12"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C45" s="14"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B46" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C46" s="18"/>
-      <c r="D46" s="12"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C46" s="14"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C47" s="18"/>
-      <c r="D47" s="12"/>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C47" s="14"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C48" s="18"/>
-      <c r="D48" s="12"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C48" s="14"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C49" s="18"/>
-      <c r="D49" s="12"/>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C49" s="14"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C50" s="19"/>
-      <c r="D50" s="12"/>
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C50" s="15"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B51" s="9"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="18" t="str">
+        <f t="shared" ref="E51:E82" si="2">IF(ISBLANK(D51),"",HYPERLINK("#'HighLevelRequirements'!B"&amp;D51,"Link"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B52" s="9"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B53" s="9"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B54" s="9"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B55" s="9"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B56" s="9"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B57" s="9"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B58" s="9"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B59" s="9"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B60" s="9"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B61" s="9"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B62" s="9"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B63" s="9"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B64" s="9"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B65" s="9"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B66" s="9"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B67" s="9"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B68" s="9"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B69" s="9"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B70" s="9"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="21"/>
+      <c r="E70" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B71" s="9"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B72" s="9"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="21"/>
+      <c r="E72" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B73" s="9"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="21"/>
+      <c r="E73" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B74" s="9"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B75" s="9"/>
+      <c r="C75" s="14"/>
+      <c r="D75" s="21"/>
+      <c r="E75" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B76" s="9"/>
+      <c r="C76" s="14"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B77" s="9"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="21"/>
+      <c r="E77" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B78" s="9"/>
+      <c r="C78" s="14"/>
+      <c r="D78" s="21"/>
+      <c r="E78" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B79" s="9"/>
+      <c r="C79" s="14"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B80" s="9"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="21"/>
+      <c r="E80" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B81" s="9"/>
+      <c r="C81" s="14"/>
+      <c r="D81" s="21"/>
+      <c r="E81" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B82" s="9"/>
+      <c r="C82" s="14"/>
+      <c r="D82" s="21"/>
+      <c r="E82" s="18" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B83" s="9"/>
+      <c r="C83" s="14"/>
+      <c r="D83" s="21"/>
+      <c r="E83" s="18" t="str">
+        <f t="shared" ref="E83:E114" si="3">IF(ISBLANK(D83),"",HYPERLINK("#'HighLevelRequirements'!B"&amp;D83,"Link"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B84" s="9"/>
+      <c r="C84" s="14"/>
+      <c r="D84" s="21"/>
+      <c r="E84" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B85" s="9"/>
+      <c r="C85" s="14"/>
+      <c r="D85" s="21"/>
+      <c r="E85" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B86" s="9"/>
+      <c r="C86" s="14"/>
+      <c r="D86" s="21"/>
+      <c r="E86" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B87" s="9"/>
+      <c r="C87" s="14"/>
+      <c r="D87" s="21"/>
+      <c r="E87" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B88" s="9"/>
+      <c r="C88" s="14"/>
+      <c r="D88" s="21"/>
+      <c r="E88" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B89" s="9"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="21"/>
+      <c r="E89" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B90" s="9"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="21"/>
+      <c r="E90" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B91" s="9"/>
+      <c r="C91" s="14"/>
+      <c r="D91" s="21"/>
+      <c r="E91" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B92" s="9"/>
+      <c r="C92" s="14"/>
+      <c r="D92" s="21"/>
+      <c r="E92" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B93" s="9"/>
+      <c r="C93" s="14"/>
+      <c r="D93" s="21"/>
+      <c r="E93" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B94" s="9"/>
+      <c r="C94" s="14"/>
+      <c r="D94" s="21"/>
+      <c r="E94" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B95" s="9"/>
+      <c r="C95" s="14"/>
+      <c r="D95" s="21"/>
+      <c r="E95" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B96" s="9"/>
+      <c r="C96" s="14"/>
+      <c r="D96" s="21"/>
+      <c r="E96" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B97" s="9"/>
+      <c r="C97" s="14"/>
+      <c r="D97" s="21"/>
+      <c r="E97" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B98" s="9"/>
+      <c r="C98" s="14"/>
+      <c r="D98" s="21"/>
+      <c r="E98" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B99" s="9"/>
+      <c r="C99" s="14"/>
+      <c r="D99" s="21"/>
+      <c r="E99" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B100" s="22"/>
+      <c r="C100" s="15"/>
+      <c r="D100" s="23"/>
+      <c r="E100" s="24" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="D4" location="'High Level Requirements'!B4" display="4" xr:uid="{1C2EECC4-2CD1-41AA-A9E1-10645D54BCCF}"/>
-    <hyperlink ref="D5" location="'High Level Requirements'!B4" display="4" xr:uid="{240E573A-F816-449B-BCAE-E640EEBE4D90}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Update Requirements. Got reverted somehow
</commit_message>
<xml_diff>
--- a/PhotonManager_Requirments.xlsx
+++ b/PhotonManager_Requirments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PhotonLaserTagManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB3422F-C698-4348-9F61-8E13AB8EAC8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{82478FFD-253F-44D8-B520-54B5D1F81540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{D1978DAF-1EAF-4D70-9253-8005321C1CD1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D1978DAF-1EAF-4D70-9253-8005321C1CD1}"/>
   </bookViews>
   <sheets>
     <sheet name="HighLevelRequirements" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Laser Tag System High-Level Requirments</t>
   </si>
@@ -66,9 +66,6 @@
     <t>The Photon Laser Tag Manager System (PLTMS) shall update the display window every 12 milliseconds (83.3Hz) in a non-blocking fashion.</t>
   </si>
   <si>
-    <t>The PLTMS shall have a resizable window, with a minimum size of (XXXX x XXXX) pixels</t>
-  </si>
-  <si>
     <t>The PLTMS shall use user keyboard inputs to fill selected text fields in the team selection screen</t>
   </si>
   <si>
@@ -81,14 +78,267 @@
     <t>The PLTMS shall be written in Java</t>
   </si>
   <si>
-    <t>The PLTMS shall be ran on a Debian virtual machine [ambiguity of whether the program is expected to run on a clean install, or if setup is allowed]</t>
+    <t>The PLTMS shall broadcast and receive data regarding player states. The software shall act as a "master server", updating all player clients.</t>
+  </si>
+  <si>
+    <t>The PLTMS shall interact with a PostgreSQL database to hold and persist all player information</t>
+  </si>
+  <si>
+    <t>The tab key shall be used to navigate fields in the UI</t>
+  </si>
+  <si>
+    <t>The PLTMS shall be built based off of the old software from the 1980's -- developers shall work to integrate new Java code to work with this old software (This is more general, no low-level requirements should be needed for this)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The PLTMS shall have a display UI, the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>game progress UI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> interfaces with the PostgreSQL database to provide the current states of the playerlist</t>
+    </r>
+  </si>
+  <si>
+    <t>NOTE: ADD THESE TASKS TO TRELLO!</t>
+  </si>
+  <si>
+    <t>The PLTMS shall have an audio class that handles the playing of audio and sfx</t>
+  </si>
+  <si>
+    <t>THE PLTMS shall have a "model" class that handles scores, active players, dead players, anything regarding the game</t>
+  </si>
+  <si>
+    <t>Create a "game log" that displays all player updates (when a player shoots another player). All this information should be received from our model</t>
+  </si>
+  <si>
+    <t>Create a points system so when players are tagged, points are added to a team via the model class</t>
+  </si>
+  <si>
+    <t>Create timer handling in our model. Once the "game-start" countdown has finished, use our networking and broadcast "202". Once the "game-end" countdown has finished, broadcast "221" three times in a row.</t>
+  </si>
+  <si>
+    <t>During any count-downs, synchronize a count-down sfx mp3 to play</t>
+  </si>
+  <si>
+    <t>During the game, play random ambience mp3 files</t>
+  </si>
+  <si>
+    <t>The F5 key shall be used to start the game in the UI</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The PLTMS shall create and bind two UDP sockets, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>broadcast on port 7500</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>receive on port 7501</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. For sending data, the program shall send only the ID of the tagged player. For receiving data, the program shall send the ID of the player who shot, and of the tagged player.</t>
+    </r>
+  </si>
+  <si>
+    <t>The PLTMS shall create and implement a PostgreSQL interface class that manages an instance of our database, create getter and setter methods for this database</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The PLTMS shall have an interactive UI, the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>player entry UI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that interfaces with the PostgreSQL database to provide the total playerlist; It may have the options to set game settings, to clear the game, and to start the game</t>
+    </r>
+  </si>
+  <si>
+    <t>[UNCLEAR/UNNECESSARY REQ] Create an update method in our networking that broadcasts to all active players their current states. On update, take all currently received data, interpret it and relay it to the game handler</t>
+  </si>
+  <si>
+    <t>Add functionality to add names to players. Ensure that these updates are relayed to the game handler</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The F1 key shall be used to clear all teams. If the game has ended, the F1 key shall return the software back to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>player entry UI</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create a count-down timer that begins with the start of the game -- display this on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">game progress UI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and have it interact with our model</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>player entry</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> screen, when adding a player, have a prompt to enter a player ID and a corresponding equipment ID. Hand these ID's over to the model for a response, if the model responds with "false", then re-prompt or skip.</t>
+    </r>
+  </si>
+  <si>
+    <t>When code "53" is received by our network update, access the model and grant 100 points to the green team -- give a stylized B besides the green team. When code "43" is received, access the model and apply the same effect but to the red team</t>
+  </si>
+  <si>
+    <t>The PLTMS shall have a resizable window, with a default size of (1000 x 800) pixels</t>
+  </si>
+  <si>
+    <t>The PLTMS shall provide functions to initialize its classes with the correct data.</t>
+  </si>
+  <si>
+    <t>The PLTMS shall be ran on a clean install of the Debian virtual machine provided for our Software Engineering class</t>
+  </si>
+  <si>
+    <t>The PLTMS shall display a 3 second splash screen on startup.</t>
+  </si>
+  <si>
+    <t>The PLTMS shall display the Photon logo as a 'splash screen'  for 3 seconds on startup. After displaying the Photon logo, the PLTMS shall enter the Player Entry Screen.</t>
+  </si>
+  <si>
+    <t>The PLTMS shall enforce the following as prerequisites to the start of any game: There is at least 1 valid player on each team, There are no duplicate Player ID's registered in the playing party, There are no duplicate Equipment ID's registered in the playing party, Every non-empty player field has a corresponding filled equipment ID field, every non-empty equipment ID field has a corresponding filled player ID field, All non-empty Player ID's are valid, and all non-empty Equipment ID's are valid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The PLTMS shall allow the user to set up 2 teams of up to 15 players per team for a laser tag game. Each player has a unique Player ID and an Equipment ID that signifies what laser equipment that player is using. </t>
+  </si>
+  <si>
+    <t>The PLTMS shall provide 'Tool Tips' that are drawn on the screen that give the user helpful information based on the state of the system.</t>
+  </si>
+  <si>
+    <t>The PLTMS shall provide a 'settings' screen, accessible from the Player Entry screen. This screen will allow the user to set UDP communication ports, the UDP address, and toggle a Debug mode.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0000"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +379,34 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -272,7 +550,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -296,9 +574,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -331,23 +606,44 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -358,49 +654,12 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -420,8 +679,42 @@
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -482,9 +775,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <numFmt numFmtId="164" formatCode="0000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -696,6 +989,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{075AD733-E70C-4BB1-93AC-CA78B944AF5C}" name="Table13" displayName="Table13" ref="B3:C100" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="B3:C100" xr:uid="{F9BD3E6F-18DE-4847-AC23-6689F47F21BF}"/>
@@ -713,8 +1010,8 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{54BA2B99-7968-4EF6-ABC0-D386B3BCB17C}" name="Requirement Number" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{1886CC6A-5D0D-42D3-BA80-3C2354B9499A}" name="Requirement Text" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{58DD8FAE-AA59-421D-A898-98D160A6E28A}" name="Parent HLR Trace" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{B8725959-29DD-4866-80D9-56BA64BCFA81}" name="Link to HLR" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{58DD8FAE-AA59-421D-A898-98D160A6E28A}" name="Parent HLR Trace" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{B8725959-29DD-4866-80D9-56BA64BCFA81}" name="Link to HLR" dataDxfId="0">
       <calculatedColumnFormula>IF(ISBLANK(D4),"",HYPERLINK("#'HighLevelRequirements'!B"&amp;D4,"Link"))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1042,29 +1339,30 @@
   <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" style="9" customWidth="1"/>
     <col min="3" max="3" width="68.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="21.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="8"/>
     </row>
     <row r="2" spans="2:11" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26"/>
+      <c r="C2" s="32"/>
     </row>
     <row r="3" spans="2:11" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
@@ -1073,577 +1371,603 @@
       <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="D3" s="24" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="2:11" ht="36" x14ac:dyDescent="0.35">
-      <c r="B4" s="9">
+      <c r="B4" s="26">
         <f>IF(ISBLANK(C4), "", ROW(B4))</f>
         <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:11" ht="36" x14ac:dyDescent="0.35">
-      <c r="B5" s="9">
+      <c r="B5" s="26">
         <f t="shared" ref="B5:B50" si="0">IF(ISBLANK(C5), "", ROW(B5))</f>
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+    </row>
+    <row r="6" spans="2:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="26">
+        <f>IF(ISBLANK(C6), "", ROW(B6))</f>
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-    </row>
-    <row r="6" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="G6" s="27" t="s">
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B7" s="26">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B7" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B8" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B9" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B10" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B11" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B12" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B13" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B14" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C14" s="4"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+    </row>
+    <row r="8" spans="2:11" ht="54" x14ac:dyDescent="0.35">
+      <c r="B8" s="26">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+    </row>
+    <row r="9" spans="2:11" ht="36" x14ac:dyDescent="0.35">
+      <c r="B9" s="26">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+    </row>
+    <row r="10" spans="2:11" ht="72" x14ac:dyDescent="0.35">
+      <c r="B10" s="26">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+    </row>
+    <row r="11" spans="2:11" ht="72" x14ac:dyDescent="0.35">
+      <c r="B11" s="26">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+    </row>
+    <row r="12" spans="2:11" ht="54" x14ac:dyDescent="0.35">
+      <c r="B12" s="26">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="36" x14ac:dyDescent="0.35">
+      <c r="B13" s="26">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="36" x14ac:dyDescent="0.35">
+      <c r="B14" s="26">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B15" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B16" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C16" s="4"/>
+      <c r="B15" s="26">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="72" x14ac:dyDescent="0.35">
+      <c r="B16" s="26">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B17" s="9" t="str">
+      <c r="B17" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C17" s="4"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B18" s="9" t="str">
+      <c r="B18" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C18" s="4"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B19" s="9" t="str">
+      <c r="B19" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B20" s="9" t="str">
+      <c r="B20" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C20" s="4"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B21" s="9" t="str">
+      <c r="B21" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C21" s="4"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B22" s="9" t="str">
+      <c r="B22" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C22" s="4"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B23" s="9" t="str">
+      <c r="B23" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C23" s="4"/>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B24" s="9" t="str">
+      <c r="B24" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C24" s="4"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B25" s="9" t="str">
+      <c r="B25" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C25" s="4"/>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B26" s="9" t="str">
+      <c r="B26" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C26" s="4"/>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B27" s="9" t="str">
+      <c r="B27" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C27" s="4"/>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B28" s="9" t="str">
+      <c r="B28" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C28" s="4"/>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B29" s="9" t="str">
+      <c r="B29" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C29" s="4"/>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B30" s="9" t="str">
+      <c r="B30" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C30" s="4"/>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B31" s="9" t="str">
+      <c r="B31" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C31" s="4"/>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B32" s="9" t="str">
+      <c r="B32" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C32" s="4"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B33" s="9" t="str">
+      <c r="B33" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C33" s="4"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B34" s="9" t="str">
+      <c r="B34" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C34" s="4"/>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B35" s="9" t="str">
+      <c r="B35" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C35" s="4"/>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B36" s="9" t="str">
+      <c r="B36" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C36" s="4"/>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B37" s="9" t="str">
+      <c r="B37" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C37" s="4"/>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B38" s="9" t="str">
+      <c r="B38" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C38" s="4"/>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B39" s="9" t="str">
+      <c r="B39" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C39" s="4"/>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B40" s="9" t="str">
+      <c r="B40" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C40" s="4"/>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B41" s="9" t="str">
+      <c r="B41" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C41" s="4"/>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B42" s="9" t="str">
+      <c r="B42" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C42" s="4"/>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B43" s="9" t="str">
+      <c r="B43" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C43" s="4"/>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B44" s="9" t="str">
+      <c r="B44" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C44" s="4"/>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B45" s="9" t="str">
+      <c r="B45" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C45" s="4"/>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B46" s="9" t="str">
+      <c r="B46" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C46" s="4"/>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B47" s="9" t="str">
+      <c r="B47" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C47" s="4"/>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B48" s="9" t="str">
+      <c r="B48" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C48" s="4"/>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B49" s="9" t="str">
+      <c r="B49" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C49" s="4"/>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B50" s="9" t="str">
+      <c r="B50" s="26" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="C50" s="7"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B51" s="9"/>
+      <c r="B51" s="26"/>
       <c r="C51" s="7"/>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B52" s="9"/>
+      <c r="B52" s="26"/>
       <c r="C52" s="7"/>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B53" s="9"/>
+      <c r="B53" s="26"/>
       <c r="C53" s="7"/>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B54" s="9"/>
+      <c r="B54" s="26"/>
       <c r="C54" s="7"/>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B55" s="9"/>
+      <c r="B55" s="26"/>
       <c r="C55" s="7"/>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B56" s="9"/>
+      <c r="B56" s="26"/>
       <c r="C56" s="7"/>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B57" s="9"/>
+      <c r="B57" s="26"/>
       <c r="C57" s="7"/>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B58" s="9"/>
+      <c r="B58" s="26"/>
       <c r="C58" s="7"/>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B59" s="9"/>
+      <c r="B59" s="26"/>
       <c r="C59" s="7"/>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B60" s="9"/>
+      <c r="B60" s="26"/>
       <c r="C60" s="7"/>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B61" s="9"/>
+      <c r="B61" s="26"/>
       <c r="C61" s="7"/>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B62" s="9"/>
+      <c r="B62" s="26"/>
       <c r="C62" s="7"/>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B63" s="9"/>
+      <c r="B63" s="26"/>
       <c r="C63" s="7"/>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B64" s="9"/>
+      <c r="B64" s="26"/>
       <c r="C64" s="7"/>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B65" s="9"/>
+      <c r="B65" s="26"/>
       <c r="C65" s="7"/>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B66" s="9"/>
+      <c r="B66" s="26"/>
       <c r="C66" s="7"/>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B67" s="9"/>
+      <c r="B67" s="26"/>
       <c r="C67" s="7"/>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B68" s="9"/>
+      <c r="B68" s="26"/>
       <c r="C68" s="7"/>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B69" s="9"/>
+      <c r="B69" s="26"/>
       <c r="C69" s="7"/>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B70" s="9"/>
+      <c r="B70" s="26"/>
       <c r="C70" s="7"/>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B71" s="9"/>
+      <c r="B71" s="26"/>
       <c r="C71" s="7"/>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B72" s="9"/>
+      <c r="B72" s="26"/>
       <c r="C72" s="7"/>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B73" s="9"/>
+      <c r="B73" s="26"/>
       <c r="C73" s="7"/>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B74" s="9"/>
+      <c r="B74" s="26"/>
       <c r="C74" s="7"/>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B75" s="9"/>
+      <c r="B75" s="26"/>
       <c r="C75" s="7"/>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B76" s="9"/>
+      <c r="B76" s="26"/>
       <c r="C76" s="7"/>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B77" s="9"/>
+      <c r="B77" s="26"/>
       <c r="C77" s="7"/>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B78" s="9"/>
+      <c r="B78" s="26"/>
       <c r="C78" s="7"/>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B79" s="9"/>
+      <c r="B79" s="26"/>
       <c r="C79" s="7"/>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B80" s="9"/>
+      <c r="B80" s="26"/>
       <c r="C80" s="7"/>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B81" s="9"/>
+      <c r="B81" s="26"/>
       <c r="C81" s="7"/>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B82" s="9"/>
+      <c r="B82" s="26"/>
       <c r="C82" s="7"/>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B83" s="9"/>
+      <c r="B83" s="26"/>
       <c r="C83" s="7"/>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B84" s="9"/>
+      <c r="B84" s="26"/>
       <c r="C84" s="7"/>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B85" s="9"/>
+      <c r="B85" s="26"/>
       <c r="C85" s="7"/>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B86" s="9"/>
+      <c r="B86" s="26"/>
       <c r="C86" s="7"/>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B87" s="9"/>
+      <c r="B87" s="26"/>
       <c r="C87" s="7"/>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B88" s="9"/>
+      <c r="B88" s="26"/>
       <c r="C88" s="7"/>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B89" s="9"/>
+      <c r="B89" s="26"/>
       <c r="C89" s="7"/>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B90" s="9"/>
+      <c r="B90" s="26"/>
       <c r="C90" s="7"/>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B91" s="9"/>
+      <c r="B91" s="26"/>
       <c r="C91" s="7"/>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B92" s="9"/>
+      <c r="B92" s="26"/>
       <c r="C92" s="7"/>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B93" s="9"/>
+      <c r="B93" s="26"/>
       <c r="C93" s="7"/>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B94" s="9"/>
+      <c r="B94" s="26"/>
       <c r="C94" s="7"/>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B95" s="9"/>
+      <c r="B95" s="26"/>
       <c r="C95" s="7"/>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B96" s="9"/>
+      <c r="B96" s="26"/>
       <c r="C96" s="7"/>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B97" s="9"/>
+      <c r="B97" s="26"/>
       <c r="C97" s="7"/>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B98" s="9"/>
+      <c r="B98" s="26"/>
       <c r="C98" s="7"/>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B99" s="9"/>
+      <c r="B99" s="26"/>
       <c r="C99" s="7"/>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B100" s="9"/>
+      <c r="B100" s="26"/>
       <c r="C100" s="7"/>
     </row>
   </sheetData>
@@ -1665,35 +1989,35 @@
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="E2" sqref="E2"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" style="10" customWidth="1"/>
-    <col min="3" max="3" width="68.33203125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="19" style="12" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="68.33203125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="19" style="11" customWidth="1"/>
     <col min="6" max="6" width="38.6640625" style="2" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="8"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="26"/>
+      <c r="C2" s="32"/>
     </row>
     <row r="3" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
@@ -1705,1040 +2029,1117 @@
       <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>5</v>
       </c>
+      <c r="F3" s="24" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="2:6" ht="54" x14ac:dyDescent="0.35">
-      <c r="B4" s="9">
-        <f>IF(ISBLANK(C4), "", ROW(B4))</f>
+      <c r="B4" s="26">
+        <f t="shared" ref="B4:B50" si="0">IF(ISBLANK(C4), "", ROW(B4))</f>
         <v>4</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="28">
         <v>4</v>
       </c>
-      <c r="E4" s="17" t="str">
-        <f t="shared" ref="E4:E50" si="0">IF(ISBLANK(D4),"",HYPERLINK("#'HighLevelRequirements'!B"&amp;D4,"Link"))</f>
+      <c r="E4" s="16" t="str">
+        <f t="shared" ref="E4:E35" si="1">IF(ISBLANK(D4),"",HYPERLINK("#'HighLevelRequirements'!B"&amp;D4,"Link"))</f>
         <v>Link</v>
       </c>
-      <c r="F4" s="19"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="2:6" ht="36" x14ac:dyDescent="0.35">
-      <c r="B5" s="9">
-        <f t="shared" ref="B5:B50" si="1">IF(ISBLANK(C5), "", ROW(B5))</f>
+      <c r="B5" s="26">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="29">
+        <v>4</v>
+      </c>
+      <c r="E5" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="36" x14ac:dyDescent="0.35">
+      <c r="B6" s="26">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="24">
-        <v>4</v>
-      </c>
-      <c r="E5" s="17" t="str">
-        <f t="shared" si="0"/>
+      <c r="D6" s="30">
+        <v>5</v>
+      </c>
+      <c r="E6" s="16" t="str">
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="36" x14ac:dyDescent="0.35">
-      <c r="B6" s="9">
+    <row r="7" spans="2:6" ht="90" x14ac:dyDescent="0.35">
+      <c r="B7" s="26">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="30">
+        <v>8</v>
+      </c>
+      <c r="E7" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="C6" s="14" t="s">
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="54" x14ac:dyDescent="0.35">
+      <c r="B8" s="26">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="30">
+        <v>9</v>
+      </c>
+      <c r="E8" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B9" s="26">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="30">
         <v>10</v>
       </c>
-      <c r="D6" s="22">
-        <v>5</v>
-      </c>
-      <c r="E6" s="17" t="str">
-        <f t="shared" si="0"/>
+      <c r="E9" s="16" t="str">
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B7" s="9">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="26">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="30">
+        <v>10</v>
+      </c>
+      <c r="E10" s="16" t="str">
         <f t="shared" si="1"/>
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="54" x14ac:dyDescent="0.35">
+      <c r="B11" s="26">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="30">
+        <v>10</v>
+      </c>
+      <c r="E11" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="72" x14ac:dyDescent="0.35">
+      <c r="B12" s="26">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="30">
+        <v>8</v>
+      </c>
+      <c r="E12" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="54" x14ac:dyDescent="0.35">
+      <c r="B13" s="26">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="30">
+        <v>12</v>
+      </c>
+      <c r="E13" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="54" x14ac:dyDescent="0.35">
+      <c r="B14" s="26">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="30">
+        <v>12</v>
+      </c>
+      <c r="E14" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="36" x14ac:dyDescent="0.35">
+      <c r="B15" s="26">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="30">
+        <v>10</v>
+      </c>
+      <c r="E15" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="36" x14ac:dyDescent="0.35">
+      <c r="B16" s="26">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="30">
+        <v>13</v>
+      </c>
+      <c r="E16" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C17" s="25"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="72" x14ac:dyDescent="0.35">
+      <c r="B18" s="26">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="30">
+        <v>13</v>
+      </c>
+      <c r="E18" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="36" x14ac:dyDescent="0.35">
+      <c r="B19" s="26">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="30">
+        <v>14</v>
+      </c>
+      <c r="E19" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B20" s="26">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="30">
+        <v>14</v>
+      </c>
+      <c r="E20" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="72" x14ac:dyDescent="0.35">
+      <c r="B21" s="26">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="30">
+        <v>10</v>
+      </c>
+      <c r="E21" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="72" x14ac:dyDescent="0.35">
+      <c r="B22" s="26">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="30">
+        <v>8</v>
+      </c>
+      <c r="E22" s="16" t="str">
+        <f t="shared" si="1"/>
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="36" x14ac:dyDescent="0.35">
+      <c r="B23" s="26">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="30">
         <v>7</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="54" x14ac:dyDescent="0.35">
-      <c r="B8" s="9">
+      <c r="E23" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="22">
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="54" x14ac:dyDescent="0.35">
+      <c r="B24" s="26">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C24" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="17" t="str">
-        <f t="shared" si="0"/>
+      <c r="D24" s="30">
+        <v>15</v>
+      </c>
+      <c r="E24" s="16" t="str">
+        <f t="shared" si="1"/>
         <v>Link</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B9" s="9" t="str">
+    <row r="25" spans="2:5" ht="144" x14ac:dyDescent="0.35">
+      <c r="B25" s="26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="30">
+        <v>16</v>
+      </c>
+      <c r="E25" s="16" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B10" s="9" t="str">
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="54" x14ac:dyDescent="0.35">
+      <c r="B26" s="26">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="30">
+        <v>10</v>
+      </c>
+      <c r="E26" s="16" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="9" t="str">
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="72" x14ac:dyDescent="0.35">
+      <c r="B27" s="26">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="30">
+        <v>10</v>
+      </c>
+      <c r="E27" s="16" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="9" t="str">
+        <v>Link</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B28" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B13" s="9" t="str">
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B29" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B14" s="9" t="str">
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B30" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B15" s="9" t="str">
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B31" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B16" s="9" t="str">
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B32" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C32" s="13"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B17" s="9" t="str">
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B33" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B18" s="9" t="str">
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B34" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C34" s="13"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B19" s="9" t="str">
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B35" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="16" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B20" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B21" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B22" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B23" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B24" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B25" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B26" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B27" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B28" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B29" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B30" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B31" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B32" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B33" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B34" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B35" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B36" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C36" s="14"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="17" t="str">
-        <f t="shared" si="0"/>
+      <c r="B36" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C36" s="13"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="16" t="str">
+        <f t="shared" ref="E36:E67" si="2">IF(ISBLANK(D36),"",HYPERLINK("#'HighLevelRequirements'!B"&amp;D36,"Link"))</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B37" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="17" t="str">
-        <f t="shared" si="0"/>
+      <c r="B37" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="16" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B38" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="17" t="str">
-        <f t="shared" si="0"/>
+      <c r="B38" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C38" s="13"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="16" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B39" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="17" t="str">
-        <f t="shared" si="0"/>
+      <c r="B39" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C39" s="13"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="16" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B40" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="17" t="str">
-        <f t="shared" si="0"/>
+      <c r="B40" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="16" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B41" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="17" t="str">
-        <f t="shared" si="0"/>
+      <c r="B41" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C41" s="13"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="16" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B42" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="17" t="str">
-        <f t="shared" si="0"/>
+      <c r="B42" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="16" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B43" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="17" t="str">
-        <f t="shared" si="0"/>
+      <c r="B43" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="16" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B44" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C44" s="14"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="17" t="str">
-        <f t="shared" si="0"/>
+      <c r="B44" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C44" s="13"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="16" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B45" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C45" s="14"/>
-      <c r="D45" s="22"/>
-      <c r="E45" s="17" t="str">
-        <f t="shared" si="0"/>
+      <c r="B45" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C45" s="13"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="16" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B46" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C46" s="14"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="17" t="str">
-        <f t="shared" si="0"/>
+      <c r="B46" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C46" s="13"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="16" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B47" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C47" s="14"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="17" t="str">
-        <f t="shared" si="0"/>
+      <c r="B47" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C47" s="13"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="16" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B48" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="22"/>
-      <c r="E48" s="17" t="str">
-        <f t="shared" si="0"/>
+      <c r="B48" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C48" s="13"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="16" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B49" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C49" s="14"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="17" t="str">
-        <f t="shared" si="0"/>
+      <c r="B49" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C49" s="13"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="16" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B50" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="22"/>
-      <c r="E50" s="17" t="str">
-        <f t="shared" si="0"/>
+      <c r="B50" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="16" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B51" s="9"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="17" t="str">
-        <f t="shared" ref="E51:E82" si="2">IF(ISBLANK(D51),"",HYPERLINK("#'HighLevelRequirements'!B"&amp;D51,"Link"))</f>
+      <c r="B51" s="26"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="30"/>
+      <c r="E51" s="16" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B52" s="9"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="17" t="str">
+      <c r="B52" s="26"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B53" s="9"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="17" t="str">
+      <c r="B53" s="26"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B54" s="9"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="22"/>
-      <c r="E54" s="17" t="str">
+      <c r="B54" s="26"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B55" s="9"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="22"/>
-      <c r="E55" s="17" t="str">
+      <c r="B55" s="26"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B56" s="9"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="22"/>
-      <c r="E56" s="17" t="str">
+      <c r="B56" s="26"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B57" s="9"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="22"/>
-      <c r="E57" s="17" t="str">
+      <c r="B57" s="26"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="30"/>
+      <c r="E57" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B58" s="9"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="22"/>
-      <c r="E58" s="17" t="str">
+      <c r="B58" s="26"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B59" s="9"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="22"/>
-      <c r="E59" s="17" t="str">
+      <c r="B59" s="26"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="30"/>
+      <c r="E59" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B60" s="9"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="22"/>
-      <c r="E60" s="17" t="str">
+      <c r="B60" s="26"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B61" s="9"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="22"/>
-      <c r="E61" s="17" t="str">
+      <c r="B61" s="26"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B62" s="9"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="22"/>
-      <c r="E62" s="17" t="str">
+      <c r="B62" s="26"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B63" s="9"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="22"/>
-      <c r="E63" s="17" t="str">
+      <c r="B63" s="26"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B64" s="9"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="22"/>
-      <c r="E64" s="17" t="str">
+      <c r="B64" s="26"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B65" s="9"/>
-      <c r="C65" s="14"/>
-      <c r="D65" s="22"/>
-      <c r="E65" s="17" t="str">
+      <c r="B65" s="26"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B66" s="9"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="22"/>
-      <c r="E66" s="17" t="str">
+      <c r="B66" s="26"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="30"/>
+      <c r="E66" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B67" s="9"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="22"/>
-      <c r="E67" s="17" t="str">
+      <c r="B67" s="26"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B68" s="9"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="22"/>
-      <c r="E68" s="17" t="str">
-        <f t="shared" si="2"/>
+      <c r="B68" s="26"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="16" t="str">
+        <f t="shared" ref="E68:E99" si="3">IF(ISBLANK(D68),"",HYPERLINK("#'HighLevelRequirements'!B"&amp;D68,"Link"))</f>
         <v/>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B69" s="9"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="22"/>
-      <c r="E69" s="17" t="str">
-        <f t="shared" si="2"/>
+      <c r="B69" s="26"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="30"/>
+      <c r="E69" s="16" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B70" s="9"/>
-      <c r="C70" s="14"/>
-      <c r="D70" s="22"/>
-      <c r="E70" s="17" t="str">
-        <f t="shared" si="2"/>
+      <c r="B70" s="26"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="16" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B71" s="9"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="22"/>
-      <c r="E71" s="17" t="str">
-        <f t="shared" si="2"/>
+      <c r="B71" s="26"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="30"/>
+      <c r="E71" s="16" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B72" s="9"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="22"/>
-      <c r="E72" s="17" t="str">
-        <f t="shared" si="2"/>
+      <c r="B72" s="26"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="30"/>
+      <c r="E72" s="16" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B73" s="9"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="22"/>
-      <c r="E73" s="17" t="str">
-        <f t="shared" si="2"/>
+      <c r="B73" s="26"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="30"/>
+      <c r="E73" s="16" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B74" s="9"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="22"/>
-      <c r="E74" s="17" t="str">
-        <f t="shared" si="2"/>
+      <c r="B74" s="26"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="30"/>
+      <c r="E74" s="16" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B75" s="9"/>
-      <c r="C75" s="14"/>
-      <c r="D75" s="22"/>
-      <c r="E75" s="17" t="str">
-        <f t="shared" si="2"/>
+      <c r="B75" s="26"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="16" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B76" s="9"/>
-      <c r="C76" s="14"/>
-      <c r="D76" s="22"/>
-      <c r="E76" s="17" t="str">
-        <f t="shared" si="2"/>
+      <c r="B76" s="26"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="30"/>
+      <c r="E76" s="16" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B77" s="9"/>
-      <c r="C77" s="14"/>
-      <c r="D77" s="22"/>
-      <c r="E77" s="17" t="str">
-        <f t="shared" si="2"/>
+      <c r="B77" s="26"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="30"/>
+      <c r="E77" s="16" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B78" s="9"/>
-      <c r="C78" s="14"/>
-      <c r="D78" s="22"/>
-      <c r="E78" s="17" t="str">
-        <f t="shared" si="2"/>
+      <c r="B78" s="26"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="30"/>
+      <c r="E78" s="16" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B79" s="9"/>
-      <c r="C79" s="14"/>
-      <c r="D79" s="22"/>
-      <c r="E79" s="17" t="str">
-        <f t="shared" si="2"/>
+      <c r="B79" s="26"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="30"/>
+      <c r="E79" s="16" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B80" s="9"/>
-      <c r="C80" s="14"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="17" t="str">
-        <f t="shared" si="2"/>
+      <c r="B80" s="26"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="30"/>
+      <c r="E80" s="16" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B81" s="9"/>
-      <c r="C81" s="14"/>
-      <c r="D81" s="22"/>
-      <c r="E81" s="17" t="str">
-        <f t="shared" si="2"/>
+      <c r="B81" s="26"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="30"/>
+      <c r="E81" s="16" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B82" s="9"/>
-      <c r="C82" s="14"/>
-      <c r="D82" s="22"/>
-      <c r="E82" s="17" t="str">
-        <f t="shared" si="2"/>
+      <c r="B82" s="26"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="30"/>
+      <c r="E82" s="16" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B83" s="9"/>
-      <c r="C83" s="14"/>
-      <c r="D83" s="22"/>
-      <c r="E83" s="17" t="str">
-        <f t="shared" ref="E83:E100" si="3">IF(ISBLANK(D83),"",HYPERLINK("#'HighLevelRequirements'!B"&amp;D83,"Link"))</f>
+      <c r="B83" s="26"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="30"/>
+      <c r="E83" s="16" t="str">
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B84" s="9"/>
-      <c r="C84" s="14"/>
-      <c r="D84" s="22"/>
-      <c r="E84" s="17" t="str">
+      <c r="B84" s="26"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="30"/>
+      <c r="E84" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B85" s="9"/>
-      <c r="C85" s="14"/>
-      <c r="D85" s="22"/>
-      <c r="E85" s="17" t="str">
+      <c r="B85" s="26"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="30"/>
+      <c r="E85" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B86" s="9"/>
-      <c r="C86" s="14"/>
-      <c r="D86" s="22"/>
-      <c r="E86" s="17" t="str">
+      <c r="B86" s="26"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="30"/>
+      <c r="E86" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B87" s="9"/>
-      <c r="C87" s="14"/>
-      <c r="D87" s="22"/>
-      <c r="E87" s="17" t="str">
+      <c r="B87" s="26"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="30"/>
+      <c r="E87" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B88" s="9"/>
-      <c r="C88" s="14"/>
-      <c r="D88" s="22"/>
-      <c r="E88" s="17" t="str">
+      <c r="B88" s="26"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="30"/>
+      <c r="E88" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B89" s="9"/>
-      <c r="C89" s="14"/>
-      <c r="D89" s="22"/>
-      <c r="E89" s="17" t="str">
+      <c r="B89" s="26"/>
+      <c r="C89" s="13"/>
+      <c r="D89" s="30"/>
+      <c r="E89" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B90" s="9"/>
-      <c r="C90" s="14"/>
-      <c r="D90" s="22"/>
-      <c r="E90" s="17" t="str">
+      <c r="B90" s="26"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="30"/>
+      <c r="E90" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B91" s="9"/>
-      <c r="C91" s="14"/>
-      <c r="D91" s="22"/>
-      <c r="E91" s="17" t="str">
+      <c r="B91" s="26"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="30"/>
+      <c r="E91" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B92" s="9"/>
-      <c r="C92" s="14"/>
-      <c r="D92" s="22"/>
-      <c r="E92" s="17" t="str">
+      <c r="B92" s="26"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="30"/>
+      <c r="E92" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B93" s="9"/>
-      <c r="C93" s="14"/>
-      <c r="D93" s="22"/>
-      <c r="E93" s="17" t="str">
+      <c r="B93" s="26"/>
+      <c r="C93" s="13"/>
+      <c r="D93" s="30"/>
+      <c r="E93" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B94" s="9"/>
-      <c r="C94" s="14"/>
-      <c r="D94" s="22"/>
-      <c r="E94" s="17" t="str">
+      <c r="B94" s="26"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="30"/>
+      <c r="E94" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B95" s="9"/>
-      <c r="C95" s="14"/>
-      <c r="D95" s="22"/>
-      <c r="E95" s="17" t="str">
+      <c r="B95" s="26"/>
+      <c r="C95" s="13"/>
+      <c r="D95" s="30"/>
+      <c r="E95" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B96" s="9"/>
-      <c r="C96" s="14"/>
-      <c r="D96" s="22"/>
-      <c r="E96" s="17" t="str">
+      <c r="B96" s="26"/>
+      <c r="C96" s="13"/>
+      <c r="D96" s="30"/>
+      <c r="E96" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B97" s="9"/>
-      <c r="C97" s="14"/>
-      <c r="D97" s="22"/>
-      <c r="E97" s="17" t="str">
+      <c r="B97" s="26"/>
+      <c r="C97" s="13"/>
+      <c r="D97" s="30"/>
+      <c r="E97" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B98" s="9"/>
-      <c r="C98" s="14"/>
-      <c r="D98" s="22"/>
-      <c r="E98" s="17" t="str">
+      <c r="B98" s="26"/>
+      <c r="C98" s="13"/>
+      <c r="D98" s="30"/>
+      <c r="E98" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B99" s="9"/>
-      <c r="C99" s="14"/>
-      <c r="D99" s="22"/>
-      <c r="E99" s="17" t="str">
+      <c r="B99" s="26"/>
+      <c r="C99" s="13"/>
+      <c r="D99" s="30"/>
+      <c r="E99" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B100" s="20"/>
-      <c r="C100" s="15"/>
-      <c r="D100" s="29"/>
-      <c r="E100" s="21" t="str">
-        <f t="shared" si="3"/>
+      <c r="B100" s="27"/>
+      <c r="C100" s="14"/>
+      <c r="D100" s="31"/>
+      <c r="E100" s="19" t="str">
+        <f t="shared" ref="E100" si="4">IF(ISBLANK(D100),"",HYPERLINK("#'HighLevelRequirements'!B"&amp;D100,"Link"))</f>
         <v/>
       </c>
     </row>
@@ -2753,4 +3154,292 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="56f02fe2-411c-4558-bf41-03a4b2b338a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100955294C2C8828448BF4A350E921A9200" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="117254b2a9fdbff1a0d6802f801aa435">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="56f02fe2-411c-4558-bf41-03a4b2b338a1" xmlns:ns4="f40e6ece-4b2a-4861-8acb-ce0d234c5c5e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7b3eb1d213dc1206b13d0cb80810c319" ns3:_="" ns4:_="">
+    <xsd:import namespace="56f02fe2-411c-4558-bf41-03a4b2b338a1"/>
+    <xsd:import namespace="f40e6ece-4b2a-4861-8acb-ce0d234c5c5e"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:_activity" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSystemTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="56f02fe2-411c-4558-bf41-03a4b2b338a1" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_activity" ma:index="11" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="15" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSystemTags" ma:index="17" nillable="true" ma:displayName="MediaServiceSystemTags" ma:hidden="true" ma:internalName="MediaServiceSystemTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="19" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="20" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="f40e6ece-4b2a-4861-8acb-ce0d234c5c5e" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="14" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E02689BC-1015-47D4-8C21-31FB63822EE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C84044A-B4D8-4E20-81B5-8600EC71C9B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="f40e6ece-4b2a-4861-8acb-ce0d234c5c5e"/>
+    <ds:schemaRef ds:uri="56f02fe2-411c-4558-bf41-03a4b2b338a1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{672EFDE7-66FA-4DAA-874A-DE50ABE54466}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="56f02fe2-411c-4558-bf41-03a4b2b338a1"/>
+    <ds:schemaRef ds:uri="f40e6ece-4b2a-4861-8acb-ce0d234c5c5e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{79c742c4-e61c-4fa5-be89-a3cb566a80d1}" enabled="0" method="" siteId="{79c742c4-e61c-4fa5-be89-a3cb566a80d1}" removed="1"/>
+</clbl:labelList>
 </file>
</xml_diff>